<commit_message>
thesis progress Aug2020 in progress
</commit_message>
<xml_diff>
--- a/8_Purchases/Sigma_Aldrich_00/TOPcandidatePolymers.xlsx
+++ b/8_Purchases/Sigma_Aldrich_00/TOPcandidatePolymers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oskat\OneDrive - Instituto Tecnologico y de Estudios Superiores de Monterrey\Documents\MNT_ITESM_Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tecmx-my.sharepoint.com/personal/a01212611_itesm_mx/Documents/Documents/MNT_ITESM_Thesis/8_Purchases/Sigma_Aldrich_00/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA1FA33-F549-4ED9-B3AD-5FAF27F1A05B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA1FA33-F549-4ED9-B3AD-5FAF27F1A05B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C74DB7A0-B3A2-4579-87BB-9DD1A019994B}"/>
+    <workbookView xWindow="6150" yWindow="1305" windowWidth="22050" windowHeight="14265" xr2:uid="{C74DB7A0-B3A2-4579-87BB-9DD1A019994B}"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2072,8 +2074,8 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>